<commit_message>
Dispatch Route authority calculation added
</commit_message>
<xml_diff>
--- a/src/CTC/Green_Line_Schedule.xlsx
+++ b/src/CTC/Green_Line_Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\TrainsRepo\ECE1140ChooChoo\src\CTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{518EACD9-4F3A-464A-B9C7-F00CE87A650D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65C5DED-7184-48D3-AA1E-C58C5B556BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{8B69A80D-850F-4154-9BF4-2347FAC8C2C8}"/>
+    <workbookView xWindow="-22065" yWindow="5640" windowWidth="21600" windowHeight="11385" xr2:uid="{8B69A80D-850F-4154-9BF4-2347FAC8C2C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Route A</t>
   </si>
@@ -65,31 +65,34 @@
     <t>Yard</t>
   </si>
   <si>
-    <t>Dormont</t>
-  </si>
-  <si>
     <t>Mt. Lebanon</t>
   </si>
   <si>
     <t>Poplar</t>
   </si>
   <si>
-    <t>Glenbury</t>
-  </si>
-  <si>
-    <t>Overbrook</t>
-  </si>
-  <si>
-    <t>Central</t>
-  </si>
-  <si>
     <t>South Bank</t>
   </si>
   <si>
-    <t>Inglewood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central </t>
+    <t>Dormont-N</t>
+  </si>
+  <si>
+    <t>Glenbury-U</t>
+  </si>
+  <si>
+    <t>Overbrook-W</t>
+  </si>
+  <si>
+    <t>Central-W</t>
+  </si>
+  <si>
+    <t>Central-I</t>
+  </si>
+  <si>
+    <t>Inglewood-I</t>
+  </si>
+  <si>
+    <t>Overbrook-I</t>
   </si>
 </sst>
 </file>
@@ -464,17 +467,18 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -488,7 +492,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -502,22 +506,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -539,10 +543,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -559,13 +563,13 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>

</xml_diff>